<commit_message>
Deltas from input file
</commit_message>
<xml_diff>
--- a/input/positions_quintet.xlsx
+++ b/input/positions_quintet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://metabcna-my.sharepoint.com/personal/amujica_caanam_com/Documents/Escritorio/exposition_tracker/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="11_AD4D2F04E46CFB4ACB3E20C87557EA90693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFD6A1D8-F0CE-4419-9085-F8BCDFF34942}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="11_AD4D2F04E46CFB4ACB3E20C87557EA90693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07D9ED63-D939-4670-BEDA-92E3936A875B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t>Description</t>
   </si>
@@ -96,22 +96,23 @@
   </si>
   <si>
     <t>UnderlyingSymbol</t>
+  </si>
+  <si>
+    <t>SEMAPA</t>
+  </si>
+  <si>
+    <t>SEM.LS</t>
+  </si>
+  <si>
+    <t>EUR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -139,13 +140,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -432,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +572,7 @@
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E6" t="s">
@@ -588,8 +585,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M19" s="2"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>